<commit_message>
aggiornato file di esempio
</commit_message>
<xml_diff>
--- a/data/data_sacca_new_datetime.xlsx
+++ b/data/data_sacca_new_datetime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\OneDrive - WB Soluzioni sas di Saccavini Andrea &amp; C\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFC288E-3A4E-4B6A-B23D-E914B26E3049}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AB160B-44F4-440C-9F32-7AF18AA9CA2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1590" yWindow="1350" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,6 +72,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d/m/yy\ h\.mm;@"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -127,8 +130,8 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -350,7 +353,7 @@
   <dimension ref="A1:G999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -358,7 +361,7 @@
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="20.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
@@ -394,10 +397,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="2">
-        <v>400</v>
+        <v>1050</v>
       </c>
-      <c r="D2" s="7">
-        <v>44110</v>
+      <c r="D2" s="8">
+        <v>44153.729166666664</v>
       </c>
       <c r="E2" s="2" t="b">
         <v>1</v>

</xml_diff>